<commit_message>
Nex excel metadata. Validation no case-sensitive. New download info
</commit_message>
<xml_diff>
--- a/app/metadata/metadataform.xlsx
+++ b/app/metadata/metadataform.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28700" windowHeight="20140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28700" windowHeight="20140" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
     <sheet name="Attribute description" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Metadata!$A$1:$V$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Metadata!$A$1:$W$1</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
   <si>
     <t>Field Name</t>
   </si>
@@ -110,9 +110,6 @@
     <t>source_note</t>
   </si>
   <si>
-    <t>Additional relevant details about the isolation source. i.e. blood, laboratory experiment or urine</t>
-  </si>
-  <si>
     <t>pathogenic</t>
   </si>
   <si>
@@ -164,6 +161,15 @@
   </si>
   <si>
     <t>The date of the sample collection. Use one of the following format: YYYY-MM-DD, YYYY-MM or YYYY</t>
+  </si>
+  <si>
+    <t>host</t>
+  </si>
+  <si>
+    <t>Additional relevant details about the isolation source.</t>
+  </si>
+  <si>
+    <t>Information about the isolation source (i.e. blood, laboratory experiment, urine...)</t>
   </si>
 </sst>
 </file>
@@ -346,7 +352,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="21">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -390,8 +396,20 @@
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -437,6 +455,9 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -450,7 +471,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -459,6 +480,8 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -467,6 +490,8 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -796,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -819,17 +844,17 @@
     <col min="13" max="13" width="15.42578125" style="8" customWidth="1"/>
     <col min="14" max="14" width="13.7109375" style="8" customWidth="1"/>
     <col min="15" max="15" width="15.5703125" style="8" customWidth="1"/>
-    <col min="16" max="16" width="20.28515625" style="8" customWidth="1"/>
-    <col min="17" max="17" width="18.28515625" style="8" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" style="8" customWidth="1"/>
-    <col min="19" max="19" width="24.7109375" style="8" customWidth="1"/>
-    <col min="20" max="20" width="18.7109375" style="8" customWidth="1"/>
-    <col min="21" max="21" width="42" style="8" customWidth="1"/>
-    <col min="22" max="22" width="35.5703125" style="8" customWidth="1"/>
-    <col min="23" max="16384" width="10.7109375" style="9"/>
+    <col min="16" max="17" width="20.28515625" style="8" customWidth="1"/>
+    <col min="18" max="18" width="18.28515625" style="8" customWidth="1"/>
+    <col min="19" max="19" width="15.42578125" style="8" customWidth="1"/>
+    <col min="20" max="20" width="24.7109375" style="8" customWidth="1"/>
+    <col min="21" max="21" width="18.7109375" style="8" customWidth="1"/>
+    <col min="22" max="22" width="42" style="8" customWidth="1"/>
+    <col min="23" max="23" width="35.5703125" style="8" customWidth="1"/>
+    <col min="24" max="16384" width="10.7109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="13" customFormat="1" ht="21" thickBot="1">
+    <row r="1" spans="1:23" s="13" customFormat="1" ht="21" thickBot="1">
       <c r="A1" s="11" t="str">
         <f>'Attribute description'!$A$3</f>
         <v>sample_name</v>
@@ -894,28 +919,31 @@
         <f>'Attribute description'!$A$18</f>
         <v>isolation_source</v>
       </c>
-      <c r="Q1" s="11" t="str">
+      <c r="Q1" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1" s="11" t="str">
         <f>'Attribute description'!$A$19</f>
         <v>source_note</v>
       </c>
-      <c r="R1" s="11" t="str">
-        <f>'Attribute description'!$A$20</f>
-        <v>pathogenic</v>
-      </c>
       <c r="S1" s="11" t="str">
         <f>'Attribute description'!$A$21</f>
+        <v>pathogenic</v>
+      </c>
+      <c r="T1" s="11" t="str">
+        <f>'Attribute description'!$A$22</f>
         <v>pathogenicity_note</v>
       </c>
-      <c r="T1" s="12" t="str">
-        <f>'Attribute description'!$A$22</f>
+      <c r="U1" s="12" t="str">
+        <f>'Attribute description'!$A$23</f>
         <v>collection_date</v>
-      </c>
-      <c r="U1" s="11" t="str">
-        <f>'Attribute description'!$A$23</f>
-        <v>collected_by</v>
       </c>
       <c r="V1" s="11" t="str">
         <f>'Attribute description'!$A$24</f>
+        <v>collected_by</v>
+      </c>
+      <c r="W1" s="11" t="str">
+        <f>'Attribute description'!$A$25</f>
         <v>notes</v>
       </c>
     </row>
@@ -933,10 +961,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -947,11 +975,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="43" customHeight="1" thickBot="1">
-      <c r="A1" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="A1" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:3" ht="24" customHeight="1" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -983,7 +1011,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="24" customHeight="1">
@@ -1005,7 +1033,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="36">
@@ -1016,7 +1044,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
@@ -1027,7 +1055,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="24" customHeight="1">
@@ -1077,8 +1105,8 @@
       <c r="B13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="16" t="s">
-        <v>44</v>
+      <c r="C13" s="17" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
@@ -1088,23 +1116,23 @@
       <c r="B14" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="16"/>
+      <c r="C14" s="17"/>
     </row>
     <row r="15" spans="1:3" ht="24" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="16"/>
+      <c r="C15" s="17"/>
     </row>
     <row r="16" spans="1:3" ht="24" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="16"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="17"/>
     </row>
     <row r="17" spans="1:3" ht="24" customHeight="1">
       <c r="A17" s="3" t="s">
@@ -1125,7 +1153,7 @@
         <v>7</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="43" customHeight="1">
@@ -1136,62 +1164,73 @@
         <v>4</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="24" customHeight="1">
-      <c r="A20" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>41</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="43" customHeight="1">
+      <c r="A20" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="24" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="24" customHeight="1">
+      <c r="A22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="43" customHeight="1">
+      <c r="A23" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="43" customHeight="1">
-      <c r="A22" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="10" t="s">
+      <c r="B23" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="24" customHeight="1">
-      <c r="A23" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>34</v>
+      <c r="C23" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="24" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>36</v>
+      <c r="C24" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="24" customHeight="1">
+      <c r="A25" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Accession id added to metadata
</commit_message>
<xml_diff>
--- a/app/metadata/metadataform.xlsx
+++ b/app/metadata/metadataform.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Attribute description" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Metadata!$A$1:$W$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Metadata!$A$1:$X$1</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
   <si>
     <t>Field Name</t>
   </si>
@@ -170,6 +170,12 @@
   </si>
   <si>
     <t>Information about the isolation source (i.e. blood, laboratory experiment, urine...)</t>
+  </si>
+  <si>
+    <t>accession_id</t>
+  </si>
+  <si>
+    <t>Unique identifier given to a DNA or protein sequence record to allow for tracking of different versions of that sequence record and the associated sequence over time in a single data repository (e.g. NCBI)</t>
   </si>
 </sst>
 </file>
@@ -352,7 +358,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="25">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -408,8 +414,20 @@
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -458,6 +476,9 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -471,7 +492,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -482,6 +503,8 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -492,6 +515,8 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -821,129 +846,132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="60.85546875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="25" style="8" customWidth="1"/>
-    <col min="5" max="5" width="21" style="8" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="8" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="8" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" style="8" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" style="8" customWidth="1"/>
-    <col min="11" max="11" width="23.140625" style="8" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" style="8" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" style="8" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" style="8" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" style="8" customWidth="1"/>
-    <col min="16" max="17" width="20.28515625" style="8" customWidth="1"/>
-    <col min="18" max="18" width="18.28515625" style="8" customWidth="1"/>
-    <col min="19" max="19" width="15.42578125" style="8" customWidth="1"/>
-    <col min="20" max="20" width="24.7109375" style="8" customWidth="1"/>
-    <col min="21" max="21" width="18.7109375" style="8" customWidth="1"/>
-    <col min="22" max="22" width="42" style="8" customWidth="1"/>
-    <col min="23" max="23" width="35.5703125" style="8" customWidth="1"/>
-    <col min="24" max="16384" width="10.7109375" style="9"/>
+    <col min="1" max="2" width="32.85546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="60.85546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="25" style="8" customWidth="1"/>
+    <col min="6" max="6" width="21" style="8" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="8" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" style="8" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" style="8" customWidth="1"/>
+    <col min="12" max="12" width="23.140625" style="8" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" style="8" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" style="8" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" style="8" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" style="8" customWidth="1"/>
+    <col min="17" max="18" width="20.28515625" style="8" customWidth="1"/>
+    <col min="19" max="19" width="18.28515625" style="8" customWidth="1"/>
+    <col min="20" max="20" width="15.42578125" style="8" customWidth="1"/>
+    <col min="21" max="21" width="24.7109375" style="8" customWidth="1"/>
+    <col min="22" max="22" width="18.7109375" style="8" customWidth="1"/>
+    <col min="23" max="23" width="42" style="8" customWidth="1"/>
+    <col min="24" max="24" width="35.5703125" style="8" customWidth="1"/>
+    <col min="25" max="16384" width="10.7109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="13" customFormat="1" ht="21" thickBot="1">
+    <row r="1" spans="1:24" s="13" customFormat="1" ht="21" thickBot="1">
       <c r="A1" s="11" t="str">
         <f>'Attribute description'!$A$3</f>
         <v>sample_name</v>
       </c>
-      <c r="B1" s="12" t="str">
-        <f>'Attribute description'!$A$4</f>
-        <v>file_names</v>
+      <c r="B1" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="C1" s="12" t="str">
         <f>'Attribute description'!$A$5</f>
-        <v>pre_assembled</v>
+        <v>file_names</v>
       </c>
       <c r="D1" s="12" t="str">
         <f>'Attribute description'!$A$6</f>
-        <v>sequencing_platform</v>
+        <v>pre_assembled</v>
       </c>
       <c r="E1" s="12" t="str">
         <f>'Attribute description'!$A$7</f>
+        <v>sequencing_platform</v>
+      </c>
+      <c r="F1" s="12" t="str">
+        <f>'Attribute description'!$A$8</f>
         <v>sequencing_type</v>
-      </c>
-      <c r="F1" s="11" t="str">
-        <f>'Attribute description'!$A$8</f>
-        <v>organism</v>
       </c>
       <c r="G1" s="11" t="str">
         <f>'Attribute description'!$A$9</f>
-        <v>strain</v>
+        <v>organism</v>
       </c>
       <c r="H1" s="11" t="str">
         <f>'Attribute description'!$A$10</f>
+        <v>strain</v>
+      </c>
+      <c r="I1" s="11" t="str">
+        <f>'Attribute description'!$A$11</f>
         <v>subtype</v>
       </c>
-      <c r="I1" s="12" t="str">
-        <f>'Attribute description'!$A$11</f>
+      <c r="J1" s="12" t="str">
+        <f>'Attribute description'!$A$12</f>
         <v>country</v>
-      </c>
-      <c r="J1" s="11" t="str">
-        <f>'Attribute description'!$A$12</f>
-        <v>region</v>
       </c>
       <c r="K1" s="11" t="str">
         <f>'Attribute description'!$A$13</f>
-        <v>city</v>
+        <v>region</v>
       </c>
       <c r="L1" s="11" t="str">
         <f>'Attribute description'!$A$14</f>
-        <v>zip_code</v>
+        <v>city</v>
       </c>
       <c r="M1" s="11" t="str">
         <f>'Attribute description'!$A$15</f>
-        <v>longitude</v>
+        <v>zip_code</v>
       </c>
       <c r="N1" s="11" t="str">
         <f>'Attribute description'!$A$16</f>
-        <v>latitude</v>
+        <v>longitude</v>
       </c>
       <c r="O1" s="11" t="str">
         <f>'Attribute description'!$A$17</f>
+        <v>latitude</v>
+      </c>
+      <c r="P1" s="11" t="str">
+        <f>'Attribute description'!$A$18</f>
         <v>location_note</v>
       </c>
-      <c r="P1" s="12" t="str">
-        <f>'Attribute description'!$A$18</f>
+      <c r="Q1" s="12" t="str">
+        <f>'Attribute description'!$A$19</f>
         <v>isolation_source</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="R1" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="11" t="str">
-        <f>'Attribute description'!$A$19</f>
+      <c r="S1" s="11" t="str">
+        <f>'Attribute description'!$A$20</f>
         <v>source_note</v>
-      </c>
-      <c r="S1" s="11" t="str">
-        <f>'Attribute description'!$A$21</f>
-        <v>pathogenic</v>
       </c>
       <c r="T1" s="11" t="str">
         <f>'Attribute description'!$A$22</f>
+        <v>pathogenic</v>
+      </c>
+      <c r="U1" s="11" t="str">
+        <f>'Attribute description'!$A$23</f>
         <v>pathogenicity_note</v>
       </c>
-      <c r="U1" s="12" t="str">
-        <f>'Attribute description'!$A$23</f>
+      <c r="V1" s="12" t="str">
+        <f>'Attribute description'!$A$24</f>
         <v>collection_date</v>
-      </c>
-      <c r="V1" s="11" t="str">
-        <f>'Attribute description'!$A$24</f>
-        <v>collected_by</v>
       </c>
       <c r="W1" s="11" t="str">
         <f>'Attribute description'!$A$25</f>
+        <v>collected_by</v>
+      </c>
+      <c r="X1" s="11" t="str">
+        <f>'Attribute description'!$A$26</f>
         <v>notes</v>
       </c>
     </row>
@@ -961,10 +989,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -975,11 +1003,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="43" customHeight="1" thickBot="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
     </row>
     <row r="2" spans="1:3" ht="24" customHeight="1" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -1003,241 +1031,252 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="43" customHeight="1">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:3" ht="54">
+      <c r="A4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="43" customHeight="1">
+      <c r="A5" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="24" customHeight="1">
-      <c r="A5" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="24" customHeight="1">
+      <c r="A6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="36">
-      <c r="A6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="36">
       <c r="A7" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="36">
+      <c r="A8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="24" customHeight="1">
-      <c r="A8" s="3" t="s">
+    <row r="9" spans="1:3" ht="24" customHeight="1">
+      <c r="A9" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="24" customHeight="1">
-      <c r="A9" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>14</v>
+      <c r="C9" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="24" customHeight="1">
-      <c r="A10" s="3" t="s">
-        <v>15</v>
+      <c r="A10" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="24" customHeight="1">
+      <c r="A11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="24" customHeight="1">
-      <c r="A11" s="5" t="s">
+    <row r="12" spans="1:3" ht="24" customHeight="1">
+      <c r="A12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B12" s="10" t="s">
         <v>7</v>
-      </c>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:3" ht="24" customHeight="1">
-      <c r="A12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>4</v>
       </c>
       <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:3" ht="24" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>43</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="17"/>
+      <c r="C14" s="18" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="15" spans="1:3" ht="24" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="17"/>
+      <c r="C15" s="18"/>
     </row>
     <row r="16" spans="1:3" ht="24" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="17"/>
+        <v>22</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="18"/>
     </row>
     <row r="17" spans="1:3" ht="24" customHeight="1">
       <c r="A17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="18"/>
+    </row>
+    <row r="18" spans="1:3" ht="24" customHeight="1">
+      <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B18" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="24" customHeight="1">
-      <c r="A18" s="5" t="s">
+    <row r="19" spans="1:3" ht="24" customHeight="1">
+      <c r="A19" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B19" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="43" customHeight="1">
-      <c r="A19" s="3" t="s">
+    <row r="20" spans="1:3" ht="43" customHeight="1">
+      <c r="A20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B20" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="43" customHeight="1">
-      <c r="A20" s="5" t="s">
+    <row r="21" spans="1:3" ht="43" customHeight="1">
+      <c r="A21" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B21" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="24" customHeight="1">
-      <c r="A21" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="24" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="24" customHeight="1">
+      <c r="A23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="43" customHeight="1">
-      <c r="A23" s="5" t="s">
+    <row r="24" spans="1:3" ht="43" customHeight="1">
+      <c r="A24" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B24" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C24" s="6" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="24" customHeight="1">
-      <c r="A24" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="24" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="24" customHeight="1">
+      <c r="A26" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="B16:B17"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Fix random assignation of metadata to files
</commit_message>
<xml_diff>
--- a/app/metadata/metadataform.xlsx
+++ b/app/metadata/metadataform.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28700" windowHeight="20140" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="37980" yWindow="0" windowWidth="33600" windowHeight="20540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -160,29 +160,99 @@
     <t>Please provide as much information as possible. Low resolution locations reduce the usability. Our recommendation is to provide either city, zip_code or longitude and latitude coordinates.</t>
   </si>
   <si>
-    <t>The date of the sample collection. Use one of the following format: YYYY-MM-DD, YYYY-MM or YYYY</t>
-  </si>
-  <si>
     <t>host</t>
   </si>
   <si>
     <t>Additional relevant details about the isolation source.</t>
   </si>
   <si>
-    <t>Information about the isolation source (i.e. blood, laboratory experiment, urine...)</t>
-  </si>
-  <si>
     <t>accession_id</t>
   </si>
   <si>
     <t>Unique identifier given to a DNA or protein sequence record to allow for tracking of different versions of that sequence record and the associated sequence over time in a single data repository (e.g. NCBI)</t>
+  </si>
+  <si>
+    <t>Information about the isolation source (i.e. blood, laboratory experiment, urine, unknown...)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The date of the sample collection. Use one of the following format: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>YYYY-MM-DD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>YYYY-MM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>YYYY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>unknown</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -269,6 +339,13 @@
       <u/>
       <sz val="14"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -427,7 +504,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -478,6 +555,9 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -885,7 +965,7 @@
         <v>sample_name</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C1" s="12" t="str">
         <f>'Attribute description'!$A$5</f>
@@ -948,7 +1028,7 @@
         <v>isolation_source</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S1" s="11" t="str">
         <f>'Attribute description'!$A$20</f>
@@ -989,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1000,14 +1080,15 @@
     <col min="1" max="1" width="29.28515625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="94.42578125" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="43" customHeight="1" thickBot="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
     </row>
     <row r="2" spans="1:3" ht="24" customHeight="1" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -1033,13 +1114,13 @@
     </row>
     <row r="4" spans="1:3" ht="54">
       <c r="A4" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="43" customHeight="1">
@@ -1144,7 +1225,7 @@
       <c r="B14" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="19" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1155,25 +1236,25 @@
       <c r="B15" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="18"/>
+      <c r="C15" s="19"/>
     </row>
     <row r="16" spans="1:3" ht="24" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="18"/>
-    </row>
-    <row r="17" spans="1:3" ht="24" customHeight="1">
+      <c r="C16" s="19"/>
+    </row>
+    <row r="17" spans="1:4" ht="24" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="18"/>
-    </row>
-    <row r="18" spans="1:3" ht="24" customHeight="1">
+      <c r="B17" s="21"/>
+      <c r="C17" s="19"/>
+    </row>
+    <row r="18" spans="1:4" ht="24" customHeight="1">
       <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
@@ -1184,7 +1265,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="24" customHeight="1">
+    <row r="19" spans="1:4" ht="24" customHeight="1">
       <c r="A19" s="5" t="s">
         <v>26</v>
       </c>
@@ -1192,10 +1273,10 @@
         <v>7</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="43" customHeight="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="43" customHeight="1">
       <c r="A20" s="3" t="s">
         <v>27</v>
       </c>
@@ -1203,12 +1284,12 @@
         <v>4</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="43" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="43" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>7</v>
@@ -1217,7 +1298,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="24" customHeight="1">
+    <row r="22" spans="1:4" ht="24" customHeight="1">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
@@ -1228,7 +1309,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="24" customHeight="1">
+    <row r="23" spans="1:4" ht="24" customHeight="1">
       <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
@@ -1239,7 +1320,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="43" customHeight="1">
+    <row r="24" spans="1:4" ht="43" customHeight="1">
       <c r="A24" s="5" t="s">
         <v>31</v>
       </c>
@@ -1247,10 +1328,11 @@
         <v>7</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="24" customHeight="1">
+        <v>49</v>
+      </c>
+      <c r="D24" s="17"/>
+    </row>
+    <row r="25" spans="1:4" ht="24" customHeight="1">
       <c r="A25" s="3" t="s">
         <v>32</v>
       </c>
@@ -1261,7 +1343,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="24" customHeight="1">
+    <row r="26" spans="1:4" ht="24" customHeight="1">
       <c r="A26" s="3" t="s">
         <v>34</v>
       </c>

</xml_diff>